<commit_message>
Added new test cases in Type Ahead service
</commit_message>
<xml_diff>
--- a/src/test/test-data/TypeAheadTestData.xlsx
+++ b/src/test/test-data/TypeAheadTestData.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="57">
   <si>
     <t>API</t>
   </si>
@@ -118,17 +118,79 @@
     <t>status=200||suggestions.keyword=bio||suggestions.keyword=methanol</t>
   </si>
   <si>
-    <t/>
-  </si>
-  <si>
-    <t>PASS</t>
+    <t>S1_TC_T6</t>
+  </si>
+  <si>
+    <t>Get Type Ahead by passing query,source and info values</t>
+  </si>
+  <si>
+    <t>/suggest</t>
+  </si>
+  <si>
+    <t>?query=bio&amp;source=wos&amp;info=sports</t>
+  </si>
+  <si>
+    <t>status=200||source=wos||suggestions.keyword=bio</t>
+  </si>
+  <si>
+    <t>/suggest/ext/act</t>
+  </si>
+  <si>
+    <t>S1_TC_T7</t>
+  </si>
+  <si>
+    <t>Get Type Ahead Suggestions for given query prefix, source and info</t>
+  </si>
+  <si>
+    <t>S1_TC_T8</t>
+  </si>
+  <si>
+    <t>/healthcheck</t>
+  </si>
+  <si>
+    <t>S1_TC_T9</t>
+  </si>
+  <si>
+    <t>To verify HealthCheck</t>
+  </si>
+  <si>
+    <t>Get Type Ahead by passing multiple sources and info values.</t>
+  </si>
+  <si>
+    <t>?query=biology&amp;source=wos&amp;info=sports&amp;size=1</t>
+  </si>
+  <si>
+    <t>S1_TC_T10</t>
+  </si>
+  <si>
+    <t>?query=biology&amp;source=wos&amp;source=categories&amp;info=sports&amp;size=1</t>
+  </si>
+  <si>
+    <t>status=200||source=wos||source=categories||suggestions.keyword=biology</t>
+  </si>
+  <si>
+    <t>Get Type Ahead Suggestions for given query prefix, multiple source values and info</t>
+  </si>
+  <si>
+    <t>status=200||source=wos||suggestions.keyword=biology</t>
+  </si>
+  <si>
+    <t>To validate Type Ahead response for invalid query params - size</t>
+  </si>
+  <si>
+    <t>?query=biology&amp;source=wos&amp;source=categories&amp;info=sports&amp;size=a</t>
+  </si>
+  <si>
+    <t>status=404</t>
+  </si>
+  <si>
+    <t>S1_TC_T11</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
   <fonts count="2">
     <font>
       <sz val="11"/>
@@ -187,7 +249,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -202,12 +264,24 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -496,26 +570,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L6"/>
+  <dimension ref="A1:L12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="L2" sqref="L2:L6"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="L12" sqref="L2:L12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="10.42578125" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="44.85546875" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="13.5703125" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="43.85546875" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="8.85546875" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="21.7109375" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="30.5703125" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" style="5" width="17.42578125" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="18.140625" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" width="50.140625" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" width="23.5703125" collapsed="true"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
+    <col min="1" max="1" width="10.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="44.85546875" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="13.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="43.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="8.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="21.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="30.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="17.42578125" style="5" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="18.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="50.140625" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="23.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12">
@@ -584,9 +658,6 @@
       <c r="K2" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="L2" t="s">
-        <v>35</v>
-      </c>
     </row>
     <row r="3" spans="1:12">
       <c r="A3" t="s">
@@ -604,8 +675,6 @@
       <c r="E3" t="s">
         <v>1</v>
       </c>
-      <c r="F3"/>
-      <c r="G3"/>
       <c r="H3"/>
       <c r="I3" t="s">
         <v>15</v>
@@ -613,10 +682,6 @@
       <c r="J3" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="K3"/>
-      <c r="L3" t="s">
-        <v>35</v>
-      </c>
     </row>
     <row r="4" spans="1:12" ht="30">
       <c r="A4" t="s">
@@ -634,16 +699,9 @@
       <c r="E4" t="s">
         <v>1</v>
       </c>
-      <c r="F4"/>
-      <c r="G4"/>
       <c r="H4"/>
-      <c r="I4"/>
       <c r="J4" s="1" t="s">
         <v>32</v>
-      </c>
-      <c r="K4"/>
-      <c r="L4" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="5" spans="1:12">
@@ -662,16 +720,9 @@
       <c r="E5" t="s">
         <v>1</v>
       </c>
-      <c r="F5"/>
-      <c r="G5"/>
       <c r="H5"/>
-      <c r="I5"/>
       <c r="J5" s="1" t="s">
         <v>33</v>
-      </c>
-      <c r="K5"/>
-      <c r="L5" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="6" spans="1:12">
@@ -690,16 +741,150 @@
       <c r="E6" t="s">
         <v>1</v>
       </c>
-      <c r="F6"/>
-      <c r="G6"/>
       <c r="H6"/>
-      <c r="I6"/>
       <c r="J6" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="K6"/>
-      <c r="L6" t="s">
+    </row>
+    <row r="7" spans="1:12" ht="30">
+      <c r="A7" t="s">
+        <v>34</v>
+      </c>
+      <c r="B7" s="6" t="s">
         <v>35</v>
+      </c>
+      <c r="C7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D7" t="s">
+        <v>36</v>
+      </c>
+      <c r="E7" t="s">
+        <v>1</v>
+      </c>
+      <c r="G7" t="s">
+        <v>37</v>
+      </c>
+      <c r="H7"/>
+      <c r="J7" s="7" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" ht="30">
+      <c r="A8" t="s">
+        <v>40</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="C8" t="s">
+        <v>21</v>
+      </c>
+      <c r="D8" t="s">
+        <v>39</v>
+      </c>
+      <c r="E8" t="s">
+        <v>1</v>
+      </c>
+      <c r="G8" t="s">
+        <v>47</v>
+      </c>
+      <c r="H8"/>
+      <c r="J8" s="7" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12">
+      <c r="A9" t="s">
+        <v>42</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="C9" t="s">
+        <v>21</v>
+      </c>
+      <c r="D9" t="s">
+        <v>43</v>
+      </c>
+      <c r="E9" t="s">
+        <v>1</v>
+      </c>
+      <c r="H9"/>
+      <c r="J9" s="7" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" ht="30">
+      <c r="A10" t="s">
+        <v>44</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="C10" t="s">
+        <v>21</v>
+      </c>
+      <c r="D10" t="s">
+        <v>39</v>
+      </c>
+      <c r="E10" t="s">
+        <v>1</v>
+      </c>
+      <c r="G10" t="s">
+        <v>49</v>
+      </c>
+      <c r="H10"/>
+      <c r="J10" s="7" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" ht="30">
+      <c r="A11" t="s">
+        <v>48</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="C11" t="s">
+        <v>21</v>
+      </c>
+      <c r="D11" t="s">
+        <v>36</v>
+      </c>
+      <c r="E11" t="s">
+        <v>1</v>
+      </c>
+      <c r="G11" t="s">
+        <v>49</v>
+      </c>
+      <c r="H11"/>
+      <c r="J11" s="7" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" ht="30">
+      <c r="A12" t="s">
+        <v>56</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="C12" t="s">
+        <v>21</v>
+      </c>
+      <c r="D12" t="s">
+        <v>39</v>
+      </c>
+      <c r="E12" t="s">
+        <v>1</v>
+      </c>
+      <c r="G12" t="s">
+        <v>54</v>
+      </c>
+      <c r="H12"/>
+      <c r="J12" s="7" t="s">
+        <v>55</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed validations failure in Type Ahead
</commit_message>
<xml_diff>
--- a/src/test/test-data/TypeAheadTestData.xlsx
+++ b/src/test/test-data/TypeAheadTestData.xlsx
@@ -208,7 +208,7 @@
     <t>Verify that Type Ahead returns  404 by passing  invalid query params - size</t>
   </si>
   <si>
-    <t>status=200||source=wos||source=categories||source=patent||source=organization||source=article||suggestions.keyword=biology</t>
+    <t>status=200||source=wos||source=categories||source=organization</t>
   </si>
 </sst>
 </file>
@@ -596,7 +596,7 @@
   <dimension ref="A1:L14"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="L14" sqref="L2:L14"/>
+      <selection activeCell="L2" sqref="L2:L14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -937,7 +937,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="14" spans="1:12" ht="45">
+    <row r="14" spans="1:12" ht="30">
       <c r="A14" t="s">
         <v>49</v>
       </c>

</xml_diff>

<commit_message>
Added Test cases into Type Ahead
</commit_message>
<xml_diff>
--- a/src/test/test-data/TypeAheadTestData.xlsx
+++ b/src/test/test-data/TypeAheadTestData.xlsx
@@ -4,18 +4,22 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15360" windowHeight="7755" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15360" windowHeight="7755"/>
   </bookViews>
   <sheets>
-    <sheet name="TypeAhesd" sheetId="1" r:id="rId1"/>
+    <sheet name="ALL" sheetId="1" r:id="rId1"/>
     <sheet name="People" sheetId="2" r:id="rId2"/>
+    <sheet name="Patents" sheetId="3" r:id="rId3"/>
+    <sheet name="Articles" sheetId="4" r:id="rId4"/>
+    <sheet name="Posts" sheetId="5" r:id="rId5"/>
+    <sheet name="Profile" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="124">
   <si>
     <t>API</t>
   </si>
@@ -56,9 +60,6 @@
     <t>?query=bio&amp;size=1</t>
   </si>
   <si>
-    <t>S1_TC_T1</t>
-  </si>
-  <si>
     <t>/search</t>
   </si>
   <si>
@@ -71,24 +72,9 @@
     <t>hits.hits._source.category</t>
   </si>
   <si>
-    <t>S1_TC_T2</t>
-  </si>
-  <si>
     <t>1PTYPEAHEAD</t>
   </si>
   <si>
-    <t>S1_TC_T3</t>
-  </si>
-  <si>
-    <t>S1_TC_T4</t>
-  </si>
-  <si>
-    <t>S1_TC_T5</t>
-  </si>
-  <si>
-    <t>/suggest/wos/(S1_TC_T1_hits.hits._source.category)</t>
-  </si>
-  <si>
     <t>/suggest/wos/mic*</t>
   </si>
   <si>
@@ -104,9 +90,6 @@
     <t>status=200||suggestions.keyword=bio||suggestions.keyword=methanol</t>
   </si>
   <si>
-    <t>S1_TC_T6</t>
-  </si>
-  <si>
     <t>/suggest</t>
   </si>
   <si>
@@ -119,21 +102,9 @@
     <t>/suggest/ext/act</t>
   </si>
   <si>
-    <t>S1_TC_T7</t>
-  </si>
-  <si>
-    <t>S1_TC_T8</t>
-  </si>
-  <si>
-    <t>S1_TC_T9</t>
-  </si>
-  <si>
     <t>?query=biology&amp;source=wos&amp;info=sports&amp;size=1</t>
   </si>
   <si>
-    <t>S1_TC_T10</t>
-  </si>
-  <si>
     <t>?query=biology&amp;source=wos&amp;source=categories&amp;info=sports&amp;size=1</t>
   </si>
   <si>
@@ -149,18 +120,9 @@
     <t>status=404</t>
   </si>
   <si>
-    <t>S1_TC_T11</t>
-  </si>
-  <si>
     <t>?query=biology</t>
   </si>
   <si>
-    <t>S1_TC_T12</t>
-  </si>
-  <si>
-    <t>S1_TC_T13</t>
-  </si>
-  <si>
     <t>?query=biology&amp;source=wos</t>
   </si>
   <si>
@@ -212,24 +174,12 @@
     <t>OPQA_1222</t>
   </si>
   <si>
-    <t>Verify that Type Ahead returns peoples by passing  query.</t>
-  </si>
-  <si>
     <t>?query=projec&amp;source=people</t>
   </si>
   <si>
-    <t>Verify that Type Ahead returns peoples by passing  user first name.</t>
-  </si>
-  <si>
     <t>?query=project&amp;source=people</t>
   </si>
   <si>
-    <t>Verify that Type Ahead returns peoples by passing  user last name.</t>
-  </si>
-  <si>
-    <t>?query=Neon1&amp;source=people</t>
-  </si>
-  <si>
     <t>status=200||source=people||suggestions.keyword=projec||suggestions.info.value=Project Neon1||suggestions.info.value=Project Neon2||suggestions.info.value=Project Neon3</t>
   </si>
   <si>
@@ -239,14 +189,215 @@
     <t>status=200||source=people||suggestions.keyword=Neon1||suggestions.info.value=Project Neon1</t>
   </si>
   <si>
-    <t>status=200||source=wos||source=people||source=categories||source=patents||source=organization||source=article||suggestions.keyword=biology</t>
+    <t>?query=biotechnology&amp;source=articles</t>
+  </si>
+  <si>
+    <t>status=200||source=articles||suggestions.keyword=biotechnology||suggestions.info.value=biotechnology</t>
+  </si>
+  <si>
+    <t>OPQA-896</t>
+  </si>
+  <si>
+    <t>Verify that to search articles for query</t>
+  </si>
+  <si>
+    <t>/wos/search</t>
+  </si>
+  <si>
+    <t>?query=biotechnology&amp;size=1&amp;fields=title,source,sortdate,abstract&amp;sort=citingsrcslocalcount:desc</t>
+  </si>
+  <si>
+    <t>hits.hits._id||hits.hits.fields.title||hits.hits.fields.abstract||hits.hits.fields.source</t>
+  </si>
+  <si>
+    <t>status=200||source=articles||suggestions.keyword=(OPQA-896_hits.hits.fields.title)||suggestions.info.value=(OPQA-896_hits.hits.fields.title)</t>
+  </si>
+  <si>
+    <t>Verify that a Type Ahead returns article suggestions  by passing  query.</t>
+  </si>
+  <si>
+    <t>Verify that Type Ahead returns article suggestions  by passing  title.</t>
+  </si>
+  <si>
+    <t>Verify that a Type Ahead returns patents suggestions  by passing  query.</t>
+  </si>
+  <si>
+    <t>?query=biotechnology&amp;source=patents</t>
+  </si>
+  <si>
+    <t>status=200||source=patents||suggestions.keyword=biotechnology||suggestions.info.value=biotechnology</t>
+  </si>
+  <si>
+    <t>OPQA-898</t>
+  </si>
+  <si>
+    <t>Verify that to get patents for query</t>
+  </si>
+  <si>
+    <t>/patents/search</t>
+  </si>
+  <si>
+    <t>?query=biotechnology&amp;size=1&amp;fields=title,patentno,sortdate,abstract,authors</t>
+  </si>
+  <si>
+    <t>hits.hits.fields.title||hits.hits.fields.patentno</t>
+  </si>
+  <si>
+    <t>status=200||source=patents||suggestions.keyword=(OPQA-898_hits.hits.fields.title)||suggestions.info.value=(OPQA-898_hits.hits.fields.title)</t>
+  </si>
+  <si>
+    <t>Verify that a Type Ahead returns patents suggestions by passing  title.</t>
+  </si>
+  <si>
+    <t>Verify that a Type Ahead returns people suggestions by passing  query.</t>
+  </si>
+  <si>
+    <t>Verify that Type Ahead returns people suggestions by passing  user last name.</t>
+  </si>
+  <si>
+    <t>Verify that Type Ahead returns people suggestions by passing  user first name.</t>
+  </si>
+  <si>
+    <t>Verify that a Type Ahead returns posts suggestions  by passing  query.</t>
+  </si>
+  <si>
+    <t>?query=post&amp;source=posts</t>
+  </si>
+  <si>
+    <t>status=200||source=posts||suggestions.keyword=post||suggestions.info.value=post</t>
+  </si>
+  <si>
+    <t>OPQA-897</t>
+  </si>
+  <si>
+    <t>Verify that user is able to search for posts</t>
+  </si>
+  <si>
+    <t>/posts/search</t>
+  </si>
+  <si>
+    <t>?query=Post&amp;size=1&amp;fields=title</t>
+  </si>
+  <si>
+    <t>hits.hits.fields.title</t>
+  </si>
+  <si>
+    <t>status=200||source=posts||suggestions.keyword=(OPQA-897_hits.hits.fields.title)||suggestions.info.value=(OPQA-897_hits.hits.fields.title)</t>
+  </si>
+  <si>
+    <t>Verify that Type Ahead returns posts suggestions  title.</t>
+  </si>
+  <si>
+    <t>Verify that a Type Ahead returns organization suggestions  by passing  query.</t>
+  </si>
+  <si>
+    <t>?query=biotechnology&amp;source=organizations</t>
+  </si>
+  <si>
+    <t>status=200||source=organizations||suggestions.keyword=biotechnology</t>
+  </si>
+  <si>
+    <t>Verify that a Type Ahead returns organization suggestions  by passing  existing organization.</t>
+  </si>
+  <si>
+    <t>/suggest/organizations/Thomson Reuters</t>
+  </si>
+  <si>
+    <t>status=200||source=organizations||suggestions.keyword=Thomson Reuters</t>
+  </si>
+  <si>
+    <t>/suggest/posts/(OPQA-897_hits.hits.fields.title)</t>
+  </si>
+  <si>
+    <t>/suggest/articles/(OPQA-896_hits.hits.fields.title)</t>
+  </si>
+  <si>
+    <t>/suggest/patents/(OPQA-898_hits.hits.fields.title)</t>
+  </si>
+  <si>
+    <t>/suggest/people/Neon1</t>
+  </si>
+  <si>
+    <t>OPQA-358</t>
+  </si>
+  <si>
+    <t>/suggest/wos/(OPQA-358_hits.hits._source.category)</t>
+  </si>
+  <si>
+    <t>status=200||source=wos||source=people||source=categories||source=organization||source=article||suggestions.keyword=biology</t>
+  </si>
+  <si>
+    <t>OPQA-736</t>
+  </si>
+  <si>
+    <t>OPQA-735</t>
+  </si>
+  <si>
+    <t>OPQA1366</t>
+  </si>
+  <si>
+    <t>OPQA1367</t>
+  </si>
+  <si>
+    <t>OPQA1368</t>
+  </si>
+  <si>
+    <t>OPQA1369</t>
+  </si>
+  <si>
+    <t>OPQA1370</t>
+  </si>
+  <si>
+    <t>OPQA1371</t>
+  </si>
+  <si>
+    <t>OPQA1372</t>
+  </si>
+  <si>
+    <t>OPQA1373</t>
+  </si>
+  <si>
+    <t>OPQA1374</t>
+  </si>
+  <si>
+    <t>OPQA1375</t>
+  </si>
+  <si>
+    <t>OPQA_1376</t>
+  </si>
+  <si>
+    <t>OPQA_1377</t>
+  </si>
+  <si>
+    <t>OPQA_1378</t>
+  </si>
+  <si>
+    <t>OPQA_1379</t>
+  </si>
+  <si>
+    <t>OPQA_1380</t>
+  </si>
+  <si>
+    <t>OPQA_1381</t>
+  </si>
+  <si>
+    <t>OPQA_1382</t>
+  </si>
+  <si>
+    <t>OPQA_1383</t>
+  </si>
+  <si>
+    <t>OPQA_1385</t>
+  </si>
+  <si>
+    <t>OPQA_1386</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -257,6 +408,20 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -301,10 +466,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top"/>
+      <protection locked="0"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -322,8 +491,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -626,19 +800,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:L14"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
       <selection activeCell="L2" sqref="L2:L14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="10.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="44.85546875" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="23" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="62.140625" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="3" max="3" width="13.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="43.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="48.42578125" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="5" max="5" width="8.85546875" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="6" max="6" width="21.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="30.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="64.140625" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="8" max="8" width="17.42578125" style="5" customWidth="1" collapsed="1"/>
     <col min="9" max="9" width="18.140625" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="10" max="10" width="50.140625" style="5" customWidth="1" collapsed="1"/>
@@ -672,7 +846,7 @@
         <v>9</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J1" s="3" t="s">
         <v>10</v>
@@ -685,17 +859,17 @@
       </c>
     </row>
     <row r="2" spans="1:12">
-      <c r="A2" t="s">
+      <c r="A2" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="B2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C2" t="s">
+        <v>49</v>
+      </c>
+      <c r="D2" t="s">
         <v>13</v>
-      </c>
-      <c r="B2" t="s">
-        <v>49</v>
-      </c>
-      <c r="C2" t="s">
-        <v>63</v>
-      </c>
-      <c r="D2" t="s">
-        <v>14</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>1</v>
@@ -707,289 +881,289 @@
       <c r="H2" s="4"/>
       <c r="I2" s="1"/>
       <c r="J2" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="K2" s="1" t="s">
         <v>16</v>
-      </c>
-      <c r="K2" s="1" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:12">
       <c r="A3" t="s">
-        <v>18</v>
+        <v>104</v>
       </c>
       <c r="B3" t="s">
-        <v>50</v>
+        <v>36</v>
       </c>
       <c r="C3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D3" t="s">
-        <v>23</v>
+        <v>100</v>
       </c>
       <c r="E3" t="s">
         <v>1</v>
       </c>
       <c r="H3"/>
       <c r="I3" t="s">
-        <v>13</v>
+        <v>99</v>
       </c>
       <c r="J3" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:12" ht="30">
       <c r="A4" t="s">
-        <v>20</v>
+        <v>105</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>52</v>
+        <v>38</v>
       </c>
       <c r="C4" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D4" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="E4" t="s">
         <v>1</v>
       </c>
       <c r="H4"/>
       <c r="J4" s="4" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
     </row>
     <row r="5" spans="1:12" ht="30">
       <c r="A5" t="s">
-        <v>21</v>
+        <v>106</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>51</v>
+        <v>37</v>
       </c>
       <c r="C5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D5" t="s">
         <v>19</v>
-      </c>
-      <c r="D5" t="s">
-        <v>25</v>
       </c>
       <c r="E5" t="s">
         <v>1</v>
       </c>
       <c r="H5"/>
       <c r="J5" s="4" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
     </row>
     <row r="6" spans="1:12" ht="30">
       <c r="A6" t="s">
-        <v>22</v>
+        <v>107</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>58</v>
+        <v>44</v>
       </c>
       <c r="C6" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D6" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="E6" t="s">
         <v>1</v>
       </c>
       <c r="H6"/>
       <c r="J6" s="4" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
     </row>
     <row r="7" spans="1:12" ht="30">
       <c r="A7" t="s">
-        <v>29</v>
+        <v>108</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>53</v>
+        <v>39</v>
       </c>
       <c r="C7" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D7" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="E7" t="s">
         <v>1</v>
       </c>
       <c r="G7" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="H7"/>
       <c r="J7" s="6" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
     </row>
     <row r="8" spans="1:12" ht="30">
       <c r="A8" t="s">
-        <v>34</v>
+        <v>109</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>59</v>
+        <v>45</v>
       </c>
       <c r="C8" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D8" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="E8" t="s">
         <v>1</v>
       </c>
       <c r="G8" t="s">
-        <v>37</v>
+        <v>27</v>
       </c>
       <c r="H8"/>
       <c r="J8" s="6" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" ht="45">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" ht="30">
       <c r="A9" t="s">
-        <v>35</v>
+        <v>110</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>60</v>
+        <v>46</v>
       </c>
       <c r="C9" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D9" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="E9" t="s">
         <v>1</v>
       </c>
       <c r="G9" t="s">
-        <v>39</v>
+        <v>28</v>
       </c>
       <c r="H9"/>
       <c r="J9" s="6" t="s">
-        <v>40</v>
+        <v>29</v>
       </c>
     </row>
     <row r="10" spans="1:12" ht="30">
       <c r="A10" t="s">
-        <v>36</v>
+        <v>111</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>54</v>
+        <v>40</v>
       </c>
       <c r="C10" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D10" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="E10" t="s">
         <v>1</v>
       </c>
       <c r="G10" t="s">
-        <v>39</v>
+        <v>28</v>
       </c>
       <c r="H10"/>
       <c r="J10" s="6" t="s">
-        <v>40</v>
+        <v>29</v>
       </c>
     </row>
     <row r="11" spans="1:12" ht="30">
       <c r="A11" t="s">
-        <v>38</v>
+        <v>103</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>61</v>
+        <v>47</v>
       </c>
       <c r="C11" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D11" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="E11" t="s">
         <v>1</v>
       </c>
       <c r="G11" t="s">
-        <v>42</v>
+        <v>31</v>
       </c>
       <c r="H11"/>
       <c r="J11" s="6" t="s">
-        <v>43</v>
+        <v>32</v>
       </c>
     </row>
     <row r="12" spans="1:12" ht="45">
       <c r="A12" t="s">
-        <v>44</v>
+        <v>112</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>55</v>
+        <v>41</v>
       </c>
       <c r="C12" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D12" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="E12" t="s">
         <v>1</v>
       </c>
       <c r="G12" t="s">
-        <v>45</v>
+        <v>33</v>
       </c>
       <c r="H12"/>
       <c r="J12" s="6" t="s">
-        <v>74</v>
+        <v>101</v>
       </c>
     </row>
     <row r="13" spans="1:12" ht="30">
       <c r="A13" t="s">
-        <v>46</v>
+        <v>113</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>56</v>
+        <v>42</v>
       </c>
       <c r="C13" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D13" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="E13" t="s">
         <v>1</v>
       </c>
       <c r="G13" t="s">
-        <v>48</v>
+        <v>34</v>
       </c>
       <c r="H13"/>
       <c r="J13" s="6" t="s">
-        <v>41</v>
+        <v>30</v>
       </c>
     </row>
     <row r="14" spans="1:12" ht="30">
       <c r="A14" t="s">
-        <v>47</v>
+        <v>102</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>57</v>
+        <v>43</v>
       </c>
       <c r="C14" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D14" t="s">
+        <v>26</v>
+      </c>
+      <c r="E14" t="s">
+        <v>1</v>
+      </c>
+      <c r="G14" t="s">
         <v>33</v>
-      </c>
-      <c r="E14" t="s">
-        <v>1</v>
-      </c>
-      <c r="G14" t="s">
-        <v>45</v>
       </c>
       <c r="H14"/>
       <c r="J14" s="6" t="s">
-        <v>62</v>
+        <v>48</v>
       </c>
     </row>
   </sheetData>
@@ -1002,7 +1176,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:L4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+    <sheetView topLeftCell="E1" workbookViewId="0">
       <selection activeCell="L2" sqref="L2:L4"/>
     </sheetView>
   </sheetViews>
@@ -1048,7 +1222,7 @@
         <v>9</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J1" s="3" t="s">
         <v>10</v>
@@ -1062,74 +1236,614 @@
     </row>
     <row r="2" spans="1:12" ht="60">
       <c r="A2" t="s">
-        <v>64</v>
+        <v>114</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>65</v>
+        <v>76</v>
       </c>
       <c r="C2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D2" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="E2" t="s">
         <v>1</v>
       </c>
       <c r="G2" t="s">
-        <v>66</v>
+        <v>51</v>
       </c>
       <c r="H2"/>
       <c r="J2" s="4" t="s">
-        <v>71</v>
+        <v>53</v>
       </c>
     </row>
     <row r="3" spans="1:12" ht="60">
       <c r="A3" t="s">
-        <v>64</v>
+        <v>115</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>67</v>
+        <v>78</v>
       </c>
       <c r="C3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D3" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="E3" t="s">
         <v>1</v>
       </c>
       <c r="G3" t="s">
-        <v>68</v>
+        <v>52</v>
       </c>
       <c r="H3"/>
       <c r="J3" s="4" t="s">
-        <v>72</v>
+        <v>54</v>
       </c>
     </row>
     <row r="4" spans="1:12" ht="30">
       <c r="A4" t="s">
-        <v>64</v>
+        <v>116</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>69</v>
+        <v>77</v>
       </c>
       <c r="C4" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D4" t="s">
-        <v>30</v>
+        <v>98</v>
       </c>
       <c r="E4" t="s">
         <v>1</v>
-      </c>
-      <c r="G4" t="s">
-        <v>70</v>
       </c>
       <c r="H4"/>
       <c r="J4" s="4" t="s">
+        <v>55</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:L4"/>
+  <sheetViews>
+    <sheetView topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="L2" sqref="L2:L4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="37.5703125" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="39.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="13.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="46.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="8.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="21.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="53.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="17.42578125" style="5" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="18.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="60.42578125" style="5" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="23.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12">
+      <c r="A1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" ht="30">
+      <c r="A2" t="s">
+        <v>117</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="C2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="E2" t="s">
+        <v>1</v>
+      </c>
+      <c r="G2" t="s">
+        <v>67</v>
+      </c>
+      <c r="H2"/>
+      <c r="J2" s="4" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" ht="30">
+      <c r="A3" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F3" s="1"/>
+      <c r="G3" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="H3" s="4"/>
+      <c r="I3" s="1"/>
+      <c r="J3" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="K3" s="4" t="s">
         <v>73</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" ht="45">
+      <c r="A4" t="s">
+        <v>118</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="C4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="E4" t="s">
+        <v>1</v>
+      </c>
+      <c r="H4"/>
+      <c r="I4" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="J4" s="4" t="s">
+        <v>74</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:L4"/>
+  <sheetViews>
+    <sheetView topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="L2" sqref="L2:L4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="37.5703125" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="39.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="13.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="46.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="8.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="21.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="53.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="17.42578125" style="5" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="18.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="60.42578125" style="5" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="23.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12">
+      <c r="A1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" ht="30">
+      <c r="A2" t="s">
+        <v>119</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="C2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="E2" t="s">
+        <v>1</v>
+      </c>
+      <c r="G2" t="s">
+        <v>56</v>
+      </c>
+      <c r="H2"/>
+      <c r="J2" s="4" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" ht="60">
+      <c r="A3" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F3" s="1"/>
+      <c r="G3" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="H3"/>
+      <c r="J3" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="K3" s="4" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" ht="45">
+      <c r="A4" t="s">
+        <v>120</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="C4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="E4" t="s">
+        <v>1</v>
+      </c>
+      <c r="H4"/>
+      <c r="I4" t="s">
+        <v>58</v>
+      </c>
+      <c r="J4" s="4" t="s">
+        <v>63</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:L4"/>
+  <sheetViews>
+    <sheetView topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="L2" sqref="L2:L4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="37.5703125" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="39.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="13.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="43.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="8.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="21.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="53.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="17.42578125" style="5" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="18.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="68.28515625" style="5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="23.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12">
+      <c r="A1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" ht="30">
+      <c r="A2" t="s">
+        <v>121</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="C2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="E2" t="s">
+        <v>1</v>
+      </c>
+      <c r="G2" t="s">
+        <v>80</v>
+      </c>
+      <c r="H2"/>
+      <c r="J2" s="4" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" ht="31.5">
+      <c r="A3" t="s">
+        <v>82</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="H3" s="4"/>
+      <c r="I3" s="1"/>
+      <c r="J3" t="s">
+        <v>15</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" ht="45">
+      <c r="A4" t="s">
+        <v>50</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="C4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>95</v>
+      </c>
+      <c r="E4" t="s">
+        <v>1</v>
+      </c>
+      <c r="H4"/>
+      <c r="I4" t="s">
+        <v>82</v>
+      </c>
+      <c r="J4" s="4" t="s">
+        <v>87</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:L3"/>
+  <sheetViews>
+    <sheetView topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="L2" sqref="L2:L3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="37.5703125" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="33.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="13.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="43.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="8.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="21.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="53.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="17.42578125" style="5" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="18.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="67.42578125" style="5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="23.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12">
+      <c r="A1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" ht="45">
+      <c r="A2" t="s">
+        <v>122</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="C2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="E2" t="s">
+        <v>1</v>
+      </c>
+      <c r="G2" t="s">
+        <v>90</v>
+      </c>
+      <c r="H2"/>
+      <c r="J2" s="4" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" ht="45">
+      <c r="A3" t="s">
+        <v>123</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="C3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="E3" t="s">
+        <v>1</v>
+      </c>
+      <c r="H3"/>
+      <c r="J3" s="4" t="s">
+        <v>94</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Modified tests in Type Ahead
</commit_message>
<xml_diff>
--- a/src/test/test-data/TypeAheadTestData.xlsx
+++ b/src/test/test-data/TypeAheadTestData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15360" windowHeight="7755"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15360" windowHeight="7755" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="ALL" sheetId="1" r:id="rId1"/>
@@ -171,9 +171,6 @@
     <t>1PSEARCHV3</t>
   </si>
   <si>
-    <t>OPQA_1222</t>
-  </si>
-  <si>
     <t>?query=projec&amp;source=people</t>
   </si>
   <si>
@@ -333,64 +330,67 @@
     <t>OPQA-735</t>
   </si>
   <si>
-    <t>OPQA1366</t>
-  </si>
-  <si>
-    <t>OPQA1367</t>
-  </si>
-  <si>
-    <t>OPQA1368</t>
-  </si>
-  <si>
-    <t>OPQA1369</t>
-  </si>
-  <si>
-    <t>OPQA1370</t>
-  </si>
-  <si>
-    <t>OPQA1371</t>
-  </si>
-  <si>
-    <t>OPQA1372</t>
-  </si>
-  <si>
-    <t>OPQA1373</t>
-  </si>
-  <si>
-    <t>OPQA1374</t>
-  </si>
-  <si>
-    <t>OPQA1375</t>
-  </si>
-  <si>
-    <t>OPQA_1376</t>
-  </si>
-  <si>
-    <t>OPQA_1377</t>
-  </si>
-  <si>
-    <t>OPQA_1378</t>
-  </si>
-  <si>
-    <t>OPQA_1379</t>
-  </si>
-  <si>
-    <t>OPQA_1380</t>
-  </si>
-  <si>
-    <t>OPQA_1381</t>
-  </si>
-  <si>
-    <t>OPQA_1382</t>
-  </si>
-  <si>
-    <t>OPQA_1383</t>
-  </si>
-  <si>
-    <t>OPQA_1385</t>
-  </si>
-  <si>
-    <t>OPQA_1386</t>
+    <t>OPQA-1366</t>
+  </si>
+  <si>
+    <t>OPQA-1367</t>
+  </si>
+  <si>
+    <t>OPQA-1368</t>
+  </si>
+  <si>
+    <t>OPQA-1369</t>
+  </si>
+  <si>
+    <t>OPQA-1370</t>
+  </si>
+  <si>
+    <t>OPQA-1371</t>
+  </si>
+  <si>
+    <t>OPQA-1372</t>
+  </si>
+  <si>
+    <t>OPQA-1373</t>
+  </si>
+  <si>
+    <t>OPQA-1374</t>
+  </si>
+  <si>
+    <t>OPQA-1375</t>
+  </si>
+  <si>
+    <t>OPQA-1376</t>
+  </si>
+  <si>
+    <t>OPQA-1377</t>
+  </si>
+  <si>
+    <t>OPQA-1378</t>
+  </si>
+  <si>
+    <t>OPQA-1379</t>
+  </si>
+  <si>
+    <t>OPQA-1380</t>
+  </si>
+  <si>
+    <t>OPQA-1381</t>
+  </si>
+  <si>
+    <t>OPQA-1382</t>
+  </si>
+  <si>
+    <t>OPQA-1383</t>
+  </si>
+  <si>
+    <t>OPQA-1384</t>
+  </si>
+  <si>
+    <t>OPQA-1385</t>
+  </si>
+  <si>
+    <t>OPQA-1386</t>
   </si>
 </sst>
 </file>
@@ -800,8 +800,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:L14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="L2" sqref="L2:L14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A12" sqref="A12:A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -860,7 +860,7 @@
     </row>
     <row r="2" spans="1:12">
       <c r="A2" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B2" t="s">
         <v>35</v>
@@ -889,7 +889,7 @@
     </row>
     <row r="3" spans="1:12">
       <c r="A3" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B3" t="s">
         <v>36</v>
@@ -898,14 +898,14 @@
         <v>17</v>
       </c>
       <c r="D3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="E3" t="s">
         <v>1</v>
       </c>
       <c r="H3"/>
       <c r="I3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="J3" s="4" t="s">
         <v>15</v>
@@ -913,7 +913,7 @@
     </row>
     <row r="4" spans="1:12" ht="30">
       <c r="A4" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>38</v>
@@ -934,7 +934,7 @@
     </row>
     <row r="5" spans="1:12" ht="30">
       <c r="A5" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>37</v>
@@ -955,7 +955,7 @@
     </row>
     <row r="6" spans="1:12" ht="30">
       <c r="A6" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B6" s="4" t="s">
         <v>44</v>
@@ -976,7 +976,7 @@
     </row>
     <row r="7" spans="1:12" ht="30">
       <c r="A7" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B7" s="6" t="s">
         <v>39</v>
@@ -1000,7 +1000,7 @@
     </row>
     <row r="8" spans="1:12" ht="30">
       <c r="A8" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B8" s="6" t="s">
         <v>45</v>
@@ -1024,7 +1024,7 @@
     </row>
     <row r="9" spans="1:12" ht="30">
       <c r="A9" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B9" s="6" t="s">
         <v>46</v>
@@ -1048,7 +1048,7 @@
     </row>
     <row r="10" spans="1:12" ht="30">
       <c r="A10" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B10" s="6" t="s">
         <v>40</v>
@@ -1072,7 +1072,7 @@
     </row>
     <row r="11" spans="1:12" ht="30">
       <c r="A11" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B11" s="6" t="s">
         <v>47</v>
@@ -1096,7 +1096,7 @@
     </row>
     <row r="12" spans="1:12" ht="45">
       <c r="A12" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B12" s="6" t="s">
         <v>41</v>
@@ -1115,12 +1115,12 @@
       </c>
       <c r="H12"/>
       <c r="J12" s="6" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="13" spans="1:12" ht="30">
       <c r="A13" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B13" s="6" t="s">
         <v>42</v>
@@ -1144,7 +1144,7 @@
     </row>
     <row r="14" spans="1:12" ht="30">
       <c r="A14" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B14" s="6" t="s">
         <v>43</v>
@@ -1176,8 +1176,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:L4"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="L2" sqref="L2:L4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1236,10 +1236,10 @@
     </row>
     <row r="2" spans="1:12" ht="60">
       <c r="A2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C2" t="s">
         <v>17</v>
@@ -1251,19 +1251,19 @@
         <v>1</v>
       </c>
       <c r="G2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="H2"/>
       <c r="J2" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="3" spans="1:12" ht="60">
       <c r="A3" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C3" t="s">
         <v>17</v>
@@ -1275,32 +1275,32 @@
         <v>1</v>
       </c>
       <c r="G3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="H3"/>
       <c r="J3" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="4" spans="1:12" ht="30">
       <c r="A4" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C4" t="s">
         <v>17</v>
       </c>
       <c r="D4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E4" t="s">
         <v>1</v>
       </c>
       <c r="H4"/>
       <c r="J4" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
   </sheetData>
@@ -1312,8 +1312,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:L4"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="L2" sqref="L2:L4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1372,10 +1372,10 @@
     </row>
     <row r="2" spans="1:12" ht="30">
       <c r="A2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C2" t="s">
         <v>17</v>
@@ -1387,32 +1387,32 @@
         <v>1</v>
       </c>
       <c r="G2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="H2"/>
       <c r="J2" s="4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="3" spans="1:12" ht="30">
       <c r="A3" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="B3" s="4" t="s">
         <v>69</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>70</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>49</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>1</v>
       </c>
       <c r="F3" s="1"/>
       <c r="G3" s="4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H3" s="4"/>
       <c r="I3" s="1"/>
@@ -1420,31 +1420,31 @@
         <v>15</v>
       </c>
       <c r="K3" s="4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="4" spans="1:12" ht="45">
       <c r="A4" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C4" t="s">
         <v>17</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E4" t="s">
         <v>1</v>
       </c>
       <c r="H4"/>
       <c r="I4" s="4" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="J4" s="4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
   </sheetData>
@@ -1456,8 +1456,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:L4"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="L2" sqref="L2:L4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1516,10 +1516,10 @@
     </row>
     <row r="2" spans="1:12" ht="30">
       <c r="A2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C2" t="s">
         <v>17</v>
@@ -1531,63 +1531,63 @@
         <v>1</v>
       </c>
       <c r="G2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H2"/>
       <c r="J2" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="3" spans="1:12" ht="60">
       <c r="A3" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="B3" s="4" t="s">
         <v>58</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>59</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>49</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>1</v>
       </c>
       <c r="F3" s="1"/>
       <c r="G3" s="5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="H3"/>
       <c r="J3" s="4" t="s">
         <v>15</v>
       </c>
       <c r="K3" s="4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="4" spans="1:12" ht="45">
       <c r="A4" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C4" t="s">
         <v>17</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E4" t="s">
         <v>1</v>
       </c>
       <c r="H4"/>
       <c r="I4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="J4" s="4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
   </sheetData>
@@ -1599,8 +1599,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:L4"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="L2" sqref="L2:L4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1659,10 +1659,10 @@
     </row>
     <row r="2" spans="1:12" ht="30">
       <c r="A2" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C2" t="s">
         <v>17</v>
@@ -1674,32 +1674,32 @@
         <v>1</v>
       </c>
       <c r="G2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="H2"/>
       <c r="J2" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="3" spans="1:12" ht="31.5">
       <c r="A3" t="s">
+        <v>81</v>
+      </c>
+      <c r="B3" s="8" t="s">
         <v>82</v>
-      </c>
-      <c r="B3" s="8" t="s">
-        <v>83</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>49</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>1</v>
       </c>
       <c r="F3" s="1"/>
       <c r="G3" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="H3" s="4"/>
       <c r="I3" s="1"/>
@@ -1707,31 +1707,31 @@
         <v>15</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="4" spans="1:12" ht="45">
       <c r="A4" t="s">
-        <v>50</v>
+        <v>121</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C4" t="s">
         <v>17</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E4" t="s">
         <v>1</v>
       </c>
       <c r="H4"/>
       <c r="I4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="J4" s="4" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
   </sheetData>
@@ -1743,8 +1743,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:L3"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="L2" sqref="L2:L3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1806,7 +1806,7 @@
         <v>122</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C2" t="s">
         <v>17</v>
@@ -1818,11 +1818,11 @@
         <v>1</v>
       </c>
       <c r="G2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="H2"/>
       <c r="J2" s="4" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="3" spans="1:12" ht="45">
@@ -1830,20 +1830,20 @@
         <v>123</v>
       </c>
       <c r="B3" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="C3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D3" s="7" t="s">
         <v>92</v>
-      </c>
-      <c r="C3" t="s">
-        <v>17</v>
-      </c>
-      <c r="D3" s="7" t="s">
-        <v>93</v>
       </c>
       <c r="E3" t="s">
         <v>1</v>
       </c>
       <c r="H3"/>
       <c r="J3" s="4" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed failing script in TypeAhead
</commit_message>
<xml_diff>
--- a/src/test/test-data/TypeAheadTestData.xlsx
+++ b/src/test/test-data/TypeAheadTestData.xlsx
@@ -177,12 +177,6 @@
     <t>?query=project&amp;source=people</t>
   </si>
   <si>
-    <t>status=200||source=people||suggestions.keyword=projec||suggestions.info.value=Project Neon1||suggestions.info.value=Project Neon2||suggestions.info.value=Project Neon3</t>
-  </si>
-  <si>
-    <t>status=200||source=people||suggestions.keyword=project||suggestions.info.value=Project Neon1||suggestions.info.value=Project Neon2||suggestions.info.value=Project Neon3</t>
-  </si>
-  <si>
     <t>status=200||source=people||suggestions.keyword=Neon1||suggestions.info.value=Project Neon1</t>
   </si>
   <si>
@@ -391,6 +385,12 @@
   </si>
   <si>
     <t>OPQA-1386</t>
+  </si>
+  <si>
+    <t>status=200||source=people||suggestions.keyword=projec||suggestions.info.value=Project Neon1||suggestions.info.value=Project Neon4||suggestions.info.value=Project Neon3</t>
+  </si>
+  <si>
+    <t>status=200||source=people||suggestions.keyword=project||suggestions.info.value=Project Neon1||suggestions.info.value=Project Neon4||suggestions.info.value=Project Neon3</t>
   </si>
 </sst>
 </file>
@@ -800,8 +800,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:L14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A12" sqref="A12:A13"/>
+    <sheetView topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="L2" sqref="L2:L14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -860,7 +860,7 @@
     </row>
     <row r="2" spans="1:12">
       <c r="A2" s="1" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B2" t="s">
         <v>35</v>
@@ -889,7 +889,7 @@
     </row>
     <row r="3" spans="1:12">
       <c r="A3" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B3" t="s">
         <v>36</v>
@@ -898,14 +898,14 @@
         <v>17</v>
       </c>
       <c r="D3" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="E3" t="s">
         <v>1</v>
       </c>
       <c r="H3"/>
       <c r="I3" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="J3" s="4" t="s">
         <v>15</v>
@@ -913,7 +913,7 @@
     </row>
     <row r="4" spans="1:12" ht="30">
       <c r="A4" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>38</v>
@@ -934,7 +934,7 @@
     </row>
     <row r="5" spans="1:12" ht="30">
       <c r="A5" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>37</v>
@@ -955,7 +955,7 @@
     </row>
     <row r="6" spans="1:12" ht="30">
       <c r="A6" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B6" s="4" t="s">
         <v>44</v>
@@ -976,7 +976,7 @@
     </row>
     <row r="7" spans="1:12" ht="30">
       <c r="A7" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B7" s="6" t="s">
         <v>39</v>
@@ -1000,7 +1000,7 @@
     </row>
     <row r="8" spans="1:12" ht="30">
       <c r="A8" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B8" s="6" t="s">
         <v>45</v>
@@ -1024,7 +1024,7 @@
     </row>
     <row r="9" spans="1:12" ht="30">
       <c r="A9" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B9" s="6" t="s">
         <v>46</v>
@@ -1048,7 +1048,7 @@
     </row>
     <row r="10" spans="1:12" ht="30">
       <c r="A10" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B10" s="6" t="s">
         <v>40</v>
@@ -1072,7 +1072,7 @@
     </row>
     <row r="11" spans="1:12" ht="30">
       <c r="A11" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B11" s="6" t="s">
         <v>47</v>
@@ -1096,7 +1096,7 @@
     </row>
     <row r="12" spans="1:12" ht="45">
       <c r="A12" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B12" s="6" t="s">
         <v>41</v>
@@ -1115,12 +1115,12 @@
       </c>
       <c r="H12"/>
       <c r="J12" s="6" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="13" spans="1:12" ht="30">
       <c r="A13" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B13" s="6" t="s">
         <v>42</v>
@@ -1144,7 +1144,7 @@
     </row>
     <row r="14" spans="1:12" ht="30">
       <c r="A14" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B14" s="6" t="s">
         <v>43</v>
@@ -1176,8 +1176,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:L4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A4"/>
+    <sheetView topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="L2" sqref="L2:L4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1236,10 +1236,10 @@
     </row>
     <row r="2" spans="1:12" ht="60">
       <c r="A2" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C2" t="s">
         <v>17</v>
@@ -1255,15 +1255,15 @@
       </c>
       <c r="H2"/>
       <c r="J2" s="4" t="s">
-        <v>52</v>
+        <v>122</v>
       </c>
     </row>
     <row r="3" spans="1:12" ht="60">
       <c r="A3" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C3" t="s">
         <v>17</v>
@@ -1279,28 +1279,28 @@
       </c>
       <c r="H3"/>
       <c r="J3" s="4" t="s">
-        <v>53</v>
+        <v>123</v>
       </c>
     </row>
     <row r="4" spans="1:12" ht="30">
       <c r="A4" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C4" t="s">
         <v>17</v>
       </c>
       <c r="D4" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="E4" t="s">
         <v>1</v>
       </c>
       <c r="H4"/>
       <c r="J4" s="4" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
   </sheetData>
@@ -1312,8 +1312,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:L4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="L2" sqref="L2:L4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1372,10 +1372,10 @@
     </row>
     <row r="2" spans="1:12" ht="30">
       <c r="A2" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C2" t="s">
         <v>17</v>
@@ -1387,32 +1387,32 @@
         <v>1</v>
       </c>
       <c r="G2" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="H2"/>
       <c r="J2" s="4" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="3" spans="1:12" ht="30">
       <c r="A3" s="4" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>49</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>1</v>
       </c>
       <c r="F3" s="1"/>
       <c r="G3" s="4" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="H3" s="4"/>
       <c r="I3" s="1"/>
@@ -1420,31 +1420,31 @@
         <v>15</v>
       </c>
       <c r="K3" s="4" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="4" spans="1:12" ht="45">
       <c r="A4" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C4" t="s">
         <v>17</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="E4" t="s">
         <v>1</v>
       </c>
       <c r="H4"/>
       <c r="I4" s="4" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="J4" s="4" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
   </sheetData>
@@ -1456,8 +1456,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:L4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="L2" sqref="L2:L4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1516,10 +1516,10 @@
     </row>
     <row r="2" spans="1:12" ht="30">
       <c r="A2" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C2" t="s">
         <v>17</v>
@@ -1531,63 +1531,63 @@
         <v>1</v>
       </c>
       <c r="G2" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="H2"/>
       <c r="J2" s="4" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="3" spans="1:12" ht="60">
       <c r="A3" s="4" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>49</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>1</v>
       </c>
       <c r="F3" s="1"/>
       <c r="G3" s="5" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="H3"/>
       <c r="J3" s="4" t="s">
         <v>15</v>
       </c>
       <c r="K3" s="4" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="4" spans="1:12" ht="45">
       <c r="A4" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C4" t="s">
         <v>17</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="E4" t="s">
         <v>1</v>
       </c>
       <c r="H4"/>
       <c r="I4" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="J4" s="4" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
   </sheetData>
@@ -1599,8 +1599,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:L4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="L2" sqref="L2:L4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1659,10 +1659,10 @@
     </row>
     <row r="2" spans="1:12" ht="30">
       <c r="A2" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C2" t="s">
         <v>17</v>
@@ -1674,32 +1674,32 @@
         <v>1</v>
       </c>
       <c r="G2" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="H2"/>
       <c r="J2" s="4" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="3" spans="1:12" ht="31.5">
       <c r="A3" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>49</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>1</v>
       </c>
       <c r="F3" s="1"/>
       <c r="G3" s="1" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="H3" s="4"/>
       <c r="I3" s="1"/>
@@ -1707,31 +1707,31 @@
         <v>15</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="4" spans="1:12" ht="45">
       <c r="A4" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C4" t="s">
         <v>17</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="E4" t="s">
         <v>1</v>
       </c>
       <c r="H4"/>
       <c r="I4" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="J4" s="4" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
   </sheetData>
@@ -1743,8 +1743,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:L3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A3"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="L2" sqref="L2:L3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1803,10 +1803,10 @@
     </row>
     <row r="2" spans="1:12" ht="45">
       <c r="A2" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C2" t="s">
         <v>17</v>
@@ -1818,32 +1818,32 @@
         <v>1</v>
       </c>
       <c r="G2" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="H2"/>
       <c r="J2" s="4" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="3" spans="1:12" ht="45">
       <c r="A3" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C3" t="s">
         <v>17</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="E3" t="s">
         <v>1</v>
       </c>
       <c r="H3"/>
       <c r="J3" s="4" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Modified TypeAhead API test case validations in TypeAhead excel sheet.
</commit_message>
<xml_diff>
--- a/src/test/test-data/TypeAheadTestData.xlsx
+++ b/src/test/test-data/TypeAheadTestData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15360" windowHeight="7755" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15360" windowHeight="7755"/>
   </bookViews>
   <sheets>
     <sheet name="ALL" sheetId="1" r:id="rId1"/>
@@ -372,10 +372,10 @@
     <t>hits.fields.title</t>
   </si>
   <si>
-    <t>status=200||source=posts||suggestions.keyword=(OPQA-897_hits.fields.title)||suggestions.info.value=(OPQA-897_hits.fields.title)</t>
-  </si>
-  <si>
-    <t>/suggest/posts/(OPQA-897_hits.fields.title)</t>
+    <t>/suggest/posts/postin</t>
+  </si>
+  <si>
+    <t>status=200||source=posts||suggestions.keyword=postin||suggestions.info.value=(OPQA-897_hits.fields.title)</t>
   </si>
 </sst>
 </file>
@@ -785,7 +785,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:L13"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
       <selection activeCell="L2" sqref="L2:L14"/>
     </sheetView>
   </sheetViews>
@@ -1560,8 +1560,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:L4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="M3" sqref="M3"/>
+    <sheetView topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="L4" sqref="L2:L4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1671,7 +1671,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="4" spans="1:12" ht="45">
+    <row r="4" spans="1:12" ht="30">
       <c r="A4" t="s">
         <v>100</v>
       </c>
@@ -1682,7 +1682,7 @@
         <v>16</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E4" t="s">
         <v>1</v>
@@ -1692,7 +1692,7 @@
         <v>68</v>
       </c>
       <c r="J4" s="4" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Modified HPA notification testcases and added to testng.xml.
</commit_message>
<xml_diff>
--- a/src/test/test-data/TypeAheadTestData.xlsx
+++ b/src/test/test-data/TypeAheadTestData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15360" windowHeight="7755"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15360" windowHeight="7755" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="ALL" sheetId="1" r:id="rId1"/>
@@ -785,7 +785,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:L13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+    <sheetView topLeftCell="E1" workbookViewId="0">
       <selection activeCell="L2" sqref="L2:L14"/>
     </sheetView>
   </sheetViews>
@@ -1704,7 +1704,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:L3"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
       <selection activeCell="L2" sqref="L2:L3"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Removed testcases from search and typeahesd module
</commit_message>
<xml_diff>
--- a/src/test/test-data/TypeAheadTestData.xlsx
+++ b/src/test/test-data/TypeAheadTestData.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent>
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bg00483545\git\1p-api-automation\src\test\test-data\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="15360" windowHeight="7755" activeTab="5"/>
   </bookViews>
@@ -19,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="253" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="103">
   <si>
     <t>API</t>
   </si>
@@ -192,21 +197,6 @@
     <t>status=200||source=patents||suggestions.keyword=biotechnology||suggestions.info.value=biotechnology</t>
   </si>
   <si>
-    <t>OPQA-898</t>
-  </si>
-  <si>
-    <t>Verify that to get patents for query</t>
-  </si>
-  <si>
-    <t>/patents/search</t>
-  </si>
-  <si>
-    <t>?query=biotechnology&amp;size=1&amp;fields=title,patentno,sortdate,abstract,authors</t>
-  </si>
-  <si>
-    <t>Verify that a Type Ahead returns patents suggestions by passing  title.</t>
-  </si>
-  <si>
     <t>Verify that a Type Ahead returns people suggestions by passing  query.</t>
   </si>
   <si>
@@ -225,21 +215,6 @@
     <t>status=200||source=posts||suggestions.keyword=post||suggestions.info.value=post</t>
   </si>
   <si>
-    <t>OPQA-897</t>
-  </si>
-  <si>
-    <t>Verify that user is able to search for posts</t>
-  </si>
-  <si>
-    <t>/posts/search</t>
-  </si>
-  <si>
-    <t>?query=Post&amp;size=1&amp;fields=title</t>
-  </si>
-  <si>
-    <t>Verify that Type Ahead returns posts suggestions  title.</t>
-  </si>
-  <si>
     <t>Verify that a Type Ahead returns organization suggestions  by passing  query.</t>
   </si>
   <si>
@@ -309,9 +284,6 @@
     <t>OPQA-1379</t>
   </si>
   <si>
-    <t>OPQA-1380</t>
-  </si>
-  <si>
     <t>OPQA-1381</t>
   </si>
   <si>
@@ -321,9 +293,6 @@
     <t>OPQA-1383</t>
   </si>
   <si>
-    <t>OPQA-1384</t>
-  </si>
-  <si>
     <t>OPQA-1385</t>
   </si>
   <si>
@@ -351,15 +320,6 @@
     <t>/suggest/wos/(OPQA-358_hits.source.category)</t>
   </si>
   <si>
-    <t>hits.fields.title||hits.fields.patentno</t>
-  </si>
-  <si>
-    <t>/suggest/patents/(OPQA-898_hits.fields.title)</t>
-  </si>
-  <si>
-    <t>status=200||source=patents||suggestions.keyword=(OPQA-898_hits.fields.title)||suggestions.info.value=(OPQA-898_hits.fields.title)</t>
-  </si>
-  <si>
     <t>hits.id||hits.fields.title||hits.fields.abstract||hits.fields.source</t>
   </si>
   <si>
@@ -369,20 +329,18 @@
     <t>status=200||source=articles||suggestions.keyword=(OPQA-896_hits.fields.title)||suggestions.info.value=(OPQA-896_hits.fields.title)</t>
   </si>
   <si>
-    <t>hits.fields.title</t>
-  </si>
-  <si>
-    <t>/suggest/posts/postin</t>
-  </si>
-  <si>
-    <t>status=200||source=posts||suggestions.keyword=postin||suggestions.info.value=(OPQA-897_hits.fields.title)</t>
+    <t/>
+  </si>
+  <si>
+    <t>PASS</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="4">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <numFmts count="0"/>
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -404,13 +362,6 @@
       <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
@@ -458,7 +409,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -477,9 +428,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -541,7 +489,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -573,9 +521,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -607,6 +556,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -782,30 +732,30 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L13"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="L2" sqref="L2:L14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="62.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="13.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="48.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="8.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="21.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="64.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="17.42578125" style="5" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="18.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="50.140625" style="5" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="23.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="23.0" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="62.140625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="13.5703125" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="48.42578125" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="8.85546875" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="21.7109375" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="64.140625" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" style="5" width="17.42578125" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="18.140625" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" style="5" width="50.140625" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="23.5703125" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>4</v>
       </c>
@@ -843,15 +793,15 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:12">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>79</v>
+        <v>69</v>
       </c>
       <c r="B2" t="s">
         <v>32</v>
       </c>
       <c r="C2" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="D2" t="s">
         <v>13</v>
@@ -869,12 +819,15 @@
         <v>15</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12">
+        <v>96</v>
+      </c>
+      <c r="L2" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>82</v>
+        <v>72</v>
       </c>
       <c r="B3" t="s">
         <v>33</v>
@@ -883,22 +836,28 @@
         <v>16</v>
       </c>
       <c r="D3" t="s">
-        <v>109</v>
+        <v>97</v>
       </c>
       <c r="E3" t="s">
         <v>1</v>
       </c>
+      <c r="F3"/>
+      <c r="G3"/>
       <c r="H3"/>
       <c r="I3" t="s">
-        <v>79</v>
+        <v>69</v>
       </c>
       <c r="J3" s="4" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="4" spans="1:12" ht="30">
+      <c r="K3"/>
+      <c r="L3" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>83</v>
+        <v>73</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>35</v>
@@ -912,14 +871,21 @@
       <c r="E4" t="s">
         <v>1</v>
       </c>
+      <c r="F4"/>
+      <c r="G4"/>
       <c r="H4"/>
+      <c r="I4"/>
       <c r="J4" s="4" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="5" spans="1:12" ht="30">
+      <c r="K4"/>
+      <c r="L4" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>84</v>
+        <v>74</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>34</v>
@@ -933,14 +899,21 @@
       <c r="E5" t="s">
         <v>1</v>
       </c>
+      <c r="F5"/>
+      <c r="G5"/>
       <c r="H5"/>
+      <c r="I5"/>
       <c r="J5" s="4" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="6" spans="1:12" ht="30">
+      <c r="K5"/>
+      <c r="L5" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>85</v>
+        <v>75</v>
       </c>
       <c r="B6" s="4" t="s">
         <v>41</v>
@@ -954,14 +927,21 @@
       <c r="E6" t="s">
         <v>1</v>
       </c>
+      <c r="F6"/>
+      <c r="G6"/>
       <c r="H6"/>
+      <c r="I6"/>
       <c r="J6" s="4" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="7" spans="1:12" ht="30">
+      <c r="K6"/>
+      <c r="L6" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>86</v>
+        <v>76</v>
       </c>
       <c r="B7" s="6" t="s">
         <v>36</v>
@@ -975,17 +955,23 @@
       <c r="E7" t="s">
         <v>1</v>
       </c>
+      <c r="F7"/>
       <c r="G7" t="s">
         <v>23</v>
       </c>
       <c r="H7"/>
+      <c r="I7"/>
       <c r="J7" s="6" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="8" spans="1:12" ht="30">
+      <c r="K7"/>
+      <c r="L7" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>87</v>
+        <v>77</v>
       </c>
       <c r="B8" s="6" t="s">
         <v>42</v>
@@ -999,17 +985,23 @@
       <c r="E8" t="s">
         <v>1</v>
       </c>
+      <c r="F8"/>
       <c r="G8" t="s">
         <v>26</v>
       </c>
       <c r="H8"/>
+      <c r="I8"/>
       <c r="J8" s="6" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="9" spans="1:12" ht="30">
+      <c r="K8"/>
+      <c r="L8" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>88</v>
+        <v>78</v>
       </c>
       <c r="B9" s="6" t="s">
         <v>43</v>
@@ -1023,17 +1015,23 @@
       <c r="E9" t="s">
         <v>1</v>
       </c>
+      <c r="F9"/>
       <c r="G9" t="s">
         <v>27</v>
       </c>
       <c r="H9"/>
+      <c r="I9"/>
       <c r="J9" s="6" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="10" spans="1:12" ht="30">
+      <c r="K9"/>
+      <c r="L9" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>89</v>
+        <v>79</v>
       </c>
       <c r="B10" s="6" t="s">
         <v>37</v>
@@ -1047,17 +1045,23 @@
       <c r="E10" t="s">
         <v>1</v>
       </c>
+      <c r="F10"/>
       <c r="G10" t="s">
         <v>27</v>
       </c>
       <c r="H10"/>
+      <c r="I10"/>
       <c r="J10" s="6" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="11" spans="1:12" ht="45">
+      <c r="K10"/>
+      <c r="L10" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>90</v>
+        <v>80</v>
       </c>
       <c r="B11" s="6" t="s">
         <v>38</v>
@@ -1071,17 +1075,23 @@
       <c r="E11" t="s">
         <v>1</v>
       </c>
+      <c r="F11"/>
       <c r="G11" t="s">
         <v>30</v>
       </c>
       <c r="H11"/>
+      <c r="I11"/>
       <c r="J11" s="6" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" ht="30">
+        <v>70</v>
+      </c>
+      <c r="K11"/>
+      <c r="L11" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>91</v>
+        <v>81</v>
       </c>
       <c r="B12" s="6" t="s">
         <v>39</v>
@@ -1095,17 +1105,23 @@
       <c r="E12" t="s">
         <v>1</v>
       </c>
+      <c r="F12"/>
       <c r="G12" t="s">
         <v>31</v>
       </c>
       <c r="H12"/>
+      <c r="I12"/>
       <c r="J12" s="6" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="13" spans="1:12" ht="30">
+      <c r="K12"/>
+      <c r="L12" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>81</v>
+        <v>71</v>
       </c>
       <c r="B13" s="6" t="s">
         <v>40</v>
@@ -1119,12 +1135,18 @@
       <c r="E13" t="s">
         <v>1</v>
       </c>
+      <c r="F13"/>
       <c r="G13" t="s">
         <v>30</v>
       </c>
       <c r="H13"/>
+      <c r="I13"/>
       <c r="J13" s="6" t="s">
         <v>15</v>
+      </c>
+      <c r="K13"/>
+      <c r="L13" t="s">
+        <v>102</v>
       </c>
     </row>
   </sheetData>
@@ -1134,30 +1156,30 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L4"/>
   <sheetViews>
     <sheetView topLeftCell="E1" workbookViewId="0">
       <selection activeCell="L4" sqref="L2:L4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="39.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="13.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="43.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="8.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="21.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="30.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="17.42578125" style="5" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="18.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="50.140625" style="5" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="23.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="11.28515625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="39.28515625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="13.5703125" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="43.85546875" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="8.85546875" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="21.7109375" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="30.5703125" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" style="5" width="17.42578125" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="18.140625" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" style="5" width="50.140625" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="23.5703125" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>4</v>
       </c>
@@ -1195,12 +1217,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="60">
+    <row r="2" spans="1:12" ht="60" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>92</v>
+        <v>82</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="C2" t="s">
         <v>16</v>
@@ -1211,20 +1233,26 @@
       <c r="E2" t="s">
         <v>1</v>
       </c>
+      <c r="F2"/>
       <c r="G2" t="s">
         <v>44</v>
       </c>
       <c r="H2"/>
+      <c r="I2"/>
       <c r="J2" s="4" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" ht="60">
+        <v>91</v>
+      </c>
+      <c r="K2"/>
+      <c r="L2" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" ht="60" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>93</v>
+        <v>83</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="C3" t="s">
         <v>16</v>
@@ -1235,33 +1263,46 @@
       <c r="E3" t="s">
         <v>1</v>
       </c>
+      <c r="F3"/>
       <c r="G3" t="s">
         <v>45</v>
       </c>
       <c r="H3"/>
+      <c r="I3"/>
       <c r="J3" s="4" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" ht="30">
+        <v>92</v>
+      </c>
+      <c r="K3"/>
+      <c r="L3" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>84</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="C4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4" t="s">
+        <v>93</v>
+      </c>
+      <c r="E4" t="s">
+        <v>1</v>
+      </c>
+      <c r="F4"/>
+      <c r="G4"/>
+      <c r="H4"/>
+      <c r="I4"/>
+      <c r="J4" s="4" t="s">
         <v>94</v>
       </c>
-      <c r="B4" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="C4" t="s">
-        <v>16</v>
-      </c>
-      <c r="D4" t="s">
-        <v>105</v>
-      </c>
-      <c r="E4" t="s">
-        <v>1</v>
-      </c>
-      <c r="H4"/>
-      <c r="J4" s="4" t="s">
-        <v>106</v>
+      <c r="K4"/>
+      <c r="L4" t="s">
+        <v>102</v>
       </c>
     </row>
   </sheetData>
@@ -1270,30 +1311,127 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:L2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" customWidth="true" width="37.5703125" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="39.28515625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="13.5703125" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="46.7109375" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="8.85546875" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="21.7109375" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="53.140625" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" style="5" width="17.42578125" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="18.140625" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" style="5" width="60.42578125" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="23.5703125" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>85</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="C2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="E2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F2"/>
+      <c r="G2" t="s">
+        <v>55</v>
+      </c>
+      <c r="H2"/>
+      <c r="I2"/>
+      <c r="J2" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="K2"/>
+      <c r="L2" t="s">
+        <v>102</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L4"/>
   <sheetViews>
     <sheetView topLeftCell="F1" workbookViewId="0">
       <selection activeCell="L4" sqref="L2:L4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="37.5703125" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="39.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="13.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="46.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="8.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="21.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="53.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="17.42578125" style="5" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="18.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="60.42578125" style="5" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="23.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="37.5703125" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="39.28515625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="13.5703125" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="46.42578125" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="8.85546875" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="21.7109375" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="53.140625" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" style="5" width="17.42578125" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="18.140625" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" style="5" width="60.42578125" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="23.5703125" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>4</v>
       </c>
@@ -1331,12 +1469,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="30">
+    <row r="2" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>95</v>
+        <v>86</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C2" t="s">
         <v>16</v>
@@ -1347,159 +1485,21 @@
       <c r="E2" t="s">
         <v>1</v>
       </c>
-      <c r="G2" t="s">
-        <v>55</v>
-      </c>
-      <c r="H2"/>
-      <c r="J2" s="4" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" ht="30">
-      <c r="A3" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="D3" s="7" t="s">
-        <v>59</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F3" s="1"/>
-      <c r="G3" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="H3" s="4"/>
-      <c r="I3" s="1"/>
-      <c r="J3" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="K3" s="4" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" ht="45">
-      <c r="A4" t="s">
-        <v>96</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="C4" t="s">
-        <v>16</v>
-      </c>
-      <c r="D4" s="7" t="s">
-        <v>111</v>
-      </c>
-      <c r="E4" t="s">
-        <v>1</v>
-      </c>
-      <c r="H4"/>
-      <c r="I4" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="J4" s="4" t="s">
-        <v>112</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L4"/>
-  <sheetViews>
-    <sheetView topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="L4" sqref="L2:L4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="37.5703125" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="39.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="13.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="46.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="8.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="21.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="53.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="17.42578125" style="5" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="18.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="60.42578125" style="5" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="23.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:12">
-      <c r="A1" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="J1" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="K1" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="L1" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" ht="30">
-      <c r="A2" t="s">
-        <v>97</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="C2" t="s">
-        <v>16</v>
-      </c>
-      <c r="D2" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="E2" t="s">
-        <v>1</v>
-      </c>
+      <c r="F2"/>
       <c r="G2" t="s">
         <v>46</v>
       </c>
       <c r="H2"/>
+      <c r="I2"/>
       <c r="J2" s="4" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="3" spans="1:12" ht="45">
+      <c r="K2"/>
+      <c r="L2" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>48</v>
       </c>
@@ -1507,7 +1507,7 @@
         <v>49</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="D3" s="7" t="s">
         <v>50</v>
@@ -1520,16 +1520,20 @@
         <v>51</v>
       </c>
       <c r="H3"/>
+      <c r="I3"/>
       <c r="J3" s="4" t="s">
         <v>15</v>
       </c>
       <c r="K3" s="4" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" ht="45">
+        <v>98</v>
+      </c>
+      <c r="L3" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>98</v>
+        <v>87</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>53</v>
@@ -1538,17 +1542,23 @@
         <v>16</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>114</v>
+        <v>99</v>
       </c>
       <c r="E4" t="s">
         <v>1</v>
       </c>
+      <c r="F4"/>
+      <c r="G4"/>
       <c r="H4"/>
       <c r="I4" t="s">
         <v>48</v>
       </c>
       <c r="J4" s="4" t="s">
-        <v>115</v>
+        <v>100</v>
+      </c>
+      <c r="K4"/>
+      <c r="L4" t="s">
+        <v>102</v>
       </c>
     </row>
   </sheetData>
@@ -1557,30 +1567,30 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:L2"/>
   <sheetViews>
-    <sheetView topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="L4" sqref="L2:L4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="37.5703125" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="39.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="13.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="43.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="8.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="21.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="53.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="17.42578125" style="5" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="18.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="68.28515625" style="5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="23.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="37.5703125" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="39.28515625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="13.5703125" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="43.85546875" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="8.85546875" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="21.7109375" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="53.140625" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" style="5" width="17.42578125" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="18.140625" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" style="5" width="68.28515625" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="23.5703125" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>4</v>
       </c>
@@ -1618,12 +1628,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="30">
+    <row r="2" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>99</v>
+        <v>88</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="C2" t="s">
         <v>16</v>
@@ -1634,65 +1644,18 @@
       <c r="E2" t="s">
         <v>1</v>
       </c>
+      <c r="F2"/>
       <c r="G2" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="H2"/>
+      <c r="I2"/>
       <c r="J2" s="4" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" ht="31.5">
-      <c r="A3" t="s">
-        <v>68</v>
-      </c>
-      <c r="B3" s="8" t="s">
-        <v>69</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="D3" s="7" t="s">
-        <v>70</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F3" s="1"/>
-      <c r="G3" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="H3" s="4"/>
-      <c r="I3" s="1"/>
-      <c r="J3" t="s">
-        <v>15</v>
-      </c>
-      <c r="K3" s="1" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" ht="30">
-      <c r="A4" t="s">
-        <v>100</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="C4" t="s">
-        <v>16</v>
-      </c>
-      <c r="D4" s="7" t="s">
-        <v>117</v>
-      </c>
-      <c r="E4" t="s">
-        <v>1</v>
-      </c>
-      <c r="H4"/>
-      <c r="I4" t="s">
-        <v>68</v>
-      </c>
-      <c r="J4" s="4" t="s">
-        <v>118</v>
+        <v>62</v>
+      </c>
+      <c r="K2"/>
+      <c r="L2" t="s">
+        <v>102</v>
       </c>
     </row>
   </sheetData>
@@ -1701,30 +1664,30 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="L2" sqref="L2:L3"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="K3" sqref="K3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="37.5703125" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="33.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="13.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="43.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="8.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="21.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="53.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="17.42578125" style="5" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="18.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="67.42578125" style="5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="23.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="37.5703125" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="33.5703125" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="13.5703125" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="43.85546875" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="8.85546875" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="21.7109375" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="53.140625" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" style="5" width="17.42578125" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="18.140625" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" style="5" width="67.42578125" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="23.5703125" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>4</v>
       </c>
@@ -1762,12 +1725,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="45">
+    <row r="2" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>101</v>
+        <v>89</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>73</v>
+        <v>63</v>
       </c>
       <c r="C2" t="s">
         <v>16</v>
@@ -1778,33 +1741,46 @@
       <c r="E2" t="s">
         <v>1</v>
       </c>
+      <c r="F2"/>
       <c r="G2" t="s">
-        <v>74</v>
+        <v>64</v>
       </c>
       <c r="H2"/>
+      <c r="I2"/>
       <c r="J2" s="4" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" ht="45">
+        <v>65</v>
+      </c>
+      <c r="K2"/>
+      <c r="L2" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>102</v>
+        <v>90</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>76</v>
+        <v>66</v>
       </c>
       <c r="C3" t="s">
         <v>16</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>77</v>
+        <v>67</v>
       </c>
       <c r="E3" t="s">
         <v>1</v>
       </c>
+      <c r="F3"/>
+      <c r="G3"/>
       <c r="H3"/>
+      <c r="I3"/>
       <c r="J3" s="4" t="s">
-        <v>78</v>
+        <v>68</v>
+      </c>
+      <c r="K3"/>
+      <c r="L3" t="s">
+        <v>102</v>
       </c>
     </row>
   </sheetData>

</xml_diff>